<commit_message>
Ver 3 - Chosing Letter Bodies
</commit_message>
<xml_diff>
--- a/4.2.2015 testing.XLSX
+++ b/4.2.2015 testing.XLSX
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\PIH-BOS-WPOZZAR\Dropbox (Beyond Nines Hosting)\wCohen\Ack Letters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wcohen\Desktop\Test Work\Ack Letters\Ver 3 - Chosing Letter Bodies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -208,9 +208,6 @@
     <t>EM1406</t>
   </si>
   <si>
-    <t>Healthy Mothers Fund</t>
-  </si>
-  <si>
     <t>????????????1383</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>In your honor</t>
   </si>
   <si>
-    <t>GN100</t>
-  </si>
-  <si>
     <t>Citizens lbx</t>
   </si>
   <si>
@@ -442,9 +436,6 @@
     <t>AG, Trib no desc</t>
   </si>
   <si>
-    <t>AG, stock, Fund</t>
-  </si>
-  <si>
     <t>AG, trib w/ desc</t>
   </si>
   <si>
@@ -469,9 +460,6 @@
     <t>ML, From IRA</t>
   </si>
   <si>
-    <t xml:space="preserve">AG, checkdate, </t>
-  </si>
-  <si>
     <t>Debug_Desc</t>
   </si>
   <si>
@@ -508,9 +496,6 @@
     <t>Apartment 4</t>
   </si>
   <si>
-    <t>AG, Trib w/ desc, Benefit Val 10, $100.37</t>
-  </si>
-  <si>
     <t>Mr. Ericksson</t>
   </si>
   <si>
@@ -526,7 +511,22 @@
     <t>ML, recurr, New donor</t>
   </si>
   <si>
-    <t>AG, Trib w/ desc, Fund, New donor</t>
+    <t>DML1503</t>
+  </si>
+  <si>
+    <t>AG, Trib w/ desc, Fund Letter, New donor</t>
+  </si>
+  <si>
+    <t>AG, Appeal Letter, Trib w/ desc, Benefit Val 10, $100.37</t>
+  </si>
+  <si>
+    <t>AG, checkdate, Acquisition</t>
+  </si>
+  <si>
+    <t>DMA1404</t>
+  </si>
+  <si>
+    <t>AG, stock, Fund Letter</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,10 +925,10 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1">
         <v>42086</v>
@@ -1056,19 +1056,19 @@
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
         <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
         <v>38</v>
@@ -1077,46 +1077,46 @@
         <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="O2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" t="s">
         <v>76</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>77</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" t="s">
         <v>78</v>
-      </c>
-      <c r="T2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" t="s">
-        <v>79</v>
       </c>
       <c r="Z2" t="s">
         <v>45</v>
       </c>
       <c r="AA2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AD2" t="s">
         <v>52</v>
       </c>
       <c r="AE2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AG2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AH2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AI2">
         <v>10</v>
@@ -1127,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1">
         <v>42006</v>
@@ -1139,13 +1139,13 @@
         <v>42006</v>
       </c>
       <c r="F3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J3" t="s">
         <v>37</v>
@@ -1157,31 +1157,31 @@
         <v>50</v>
       </c>
       <c r="N3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P3" t="s">
         <v>101</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>102</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>103</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
         <v>104</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>105</v>
-      </c>
-      <c r="U3" t="s">
-        <v>106</v>
-      </c>
-      <c r="V3" t="s">
-        <v>107</v>
       </c>
       <c r="Z3" t="s">
         <v>45</v>
       </c>
       <c r="AA3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AD3" t="s">
         <v>52</v>
@@ -1192,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C4" s="1">
         <v>41987</v>
@@ -1213,49 +1213,49 @@
         <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
         <v>49</v>
       </c>
       <c r="M4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N4" t="s">
         <v>51</v>
       </c>
       <c r="O4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" t="s">
         <v>64</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>66</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>67</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>68</v>
-      </c>
-      <c r="V4" t="s">
-        <v>69</v>
       </c>
       <c r="Z4" t="s">
         <v>45</v>
       </c>
       <c r="AA4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AD4" t="s">
         <v>52</v>
       </c>
       <c r="AJ4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="AK4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -1263,7 +1263,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" s="1">
         <v>41980</v>
@@ -1281,7 +1281,7 @@
         <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J5" t="s">
         <v>37</v>
@@ -1293,7 +1293,7 @@
         <v>49</v>
       </c>
       <c r="M5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N5" t="s">
         <v>51</v>
@@ -1331,7 +1331,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1">
         <v>41978</v>
@@ -1343,7 +1343,7 @@
         <v>41978</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H6" t="s">
         <v>47</v>
@@ -1352,7 +1352,7 @@
         <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
         <v>38</v>
@@ -1364,28 +1364,28 @@
         <v>51</v>
       </c>
       <c r="O6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" t="s">
         <v>76</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
+        <v>66</v>
+      </c>
+      <c r="U6" t="s">
+        <v>67</v>
+      </c>
+      <c r="V6" t="s">
         <v>78</v>
-      </c>
-      <c r="T6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U6" t="s">
-        <v>68</v>
-      </c>
-      <c r="V6" t="s">
-        <v>79</v>
       </c>
       <c r="Z6" t="s">
         <v>45</v>
       </c>
       <c r="AA6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AD6" t="s">
         <v>52</v>
@@ -1396,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C7" s="1">
         <v>41975</v>
@@ -1411,19 +1411,19 @@
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
         <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
         <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L7" t="s">
         <v>38</v>
@@ -1432,49 +1432,49 @@
         <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O7" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q7" t="s">
         <v>89</v>
       </c>
-      <c r="P7" t="s">
+      <c r="T7" t="s">
         <v>90</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="U7" t="s">
+        <v>86</v>
+      </c>
+      <c r="V7" t="s">
         <v>91</v>
-      </c>
-      <c r="T7" t="s">
-        <v>92</v>
-      </c>
-      <c r="U7" t="s">
-        <v>88</v>
-      </c>
-      <c r="V7" t="s">
-        <v>93</v>
       </c>
       <c r="Z7" t="s">
         <v>45</v>
       </c>
       <c r="AA7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG7" t="s">
         <v>94</v>
       </c>
-      <c r="AD7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>95</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>96</v>
-      </c>
       <c r="AH7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AJ7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C8" s="1">
         <v>41945</v>
@@ -1497,19 +1497,19 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
         <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
         <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L8" t="s">
         <v>38</v>
@@ -1518,31 +1518,31 @@
         <v>50</v>
       </c>
       <c r="N8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q8" t="s">
         <v>89</v>
       </c>
-      <c r="P8" t="s">
+      <c r="T8" t="s">
         <v>90</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="U8" t="s">
+        <v>86</v>
+      </c>
+      <c r="V8" t="s">
         <v>91</v>
-      </c>
-      <c r="T8" t="s">
-        <v>92</v>
-      </c>
-      <c r="U8" t="s">
-        <v>88</v>
-      </c>
-      <c r="V8" t="s">
-        <v>93</v>
       </c>
       <c r="Z8" t="s">
         <v>45</v>
       </c>
       <c r="AA8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AD8" t="s">
         <v>52</v>
@@ -1553,7 +1553,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C9" s="1">
         <v>41940</v>
@@ -1574,7 +1574,7 @@
         <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L9" t="s">
         <v>49</v>
@@ -1583,43 +1583,43 @@
         <v>50</v>
       </c>
       <c r="N9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Q9" t="s">
+        <v>111</v>
+      </c>
+      <c r="T9" t="s">
+        <v>112</v>
+      </c>
+      <c r="U9" t="s">
+        <v>67</v>
+      </c>
+      <c r="V9" t="s">
         <v>113</v>
       </c>
-      <c r="T9" t="s">
-        <v>114</v>
-      </c>
-      <c r="U9" t="s">
-        <v>68</v>
-      </c>
-      <c r="V9" t="s">
-        <v>115</v>
-      </c>
       <c r="X9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Y9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Z9" t="s">
         <v>45</v>
       </c>
       <c r="AA9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AB9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AD9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C10" s="1">
         <v>41940</v>
@@ -1648,7 +1648,7 @@
         <v>37</v>
       </c>
       <c r="K10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L10" t="s">
         <v>49</v>
@@ -1657,37 +1657,37 @@
         <v>50</v>
       </c>
       <c r="N10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Q10" t="s">
+        <v>111</v>
+      </c>
+      <c r="T10" t="s">
+        <v>112</v>
+      </c>
+      <c r="U10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" t="s">
         <v>113</v>
-      </c>
-      <c r="T10" t="s">
-        <v>114</v>
-      </c>
-      <c r="U10" t="s">
-        <v>68</v>
-      </c>
-      <c r="V10" t="s">
-        <v>115</v>
       </c>
       <c r="Z10" t="s">
         <v>45</v>
       </c>
       <c r="AA10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AB10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AD10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C11" s="1">
         <v>41819</v>
@@ -1707,16 +1707,16 @@
         <v>41819</v>
       </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H11" t="s">
         <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L11" t="s">
         <v>49</v>
@@ -1752,7 +1752,7 @@
         <v>59</v>
       </c>
       <c r="AD11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -1760,7 +1760,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C12" s="1">
         <v>41766</v>
@@ -1775,19 +1775,19 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
         <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s">
         <v>37</v>
       </c>
       <c r="K12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L12" t="s">
         <v>49</v>
@@ -1796,46 +1796,46 @@
         <v>50</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O12" t="s">
+        <v>109</v>
+      </c>
+      <c r="P12" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q12" t="s">
         <v>111</v>
       </c>
-      <c r="P12" t="s">
+      <c r="T12" t="s">
         <v>112</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="U12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" t="s">
         <v>113</v>
-      </c>
-      <c r="T12" t="s">
-        <v>114</v>
-      </c>
-      <c r="U12" t="s">
-        <v>68</v>
-      </c>
-      <c r="V12" t="s">
-        <v>115</v>
       </c>
       <c r="Z12" t="s">
         <v>45</v>
       </c>
       <c r="AA12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AD12" t="s">
         <v>52</v>
       </c>
       <c r="AE12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AF12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AG12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AH12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1">
         <v>41721</v>
@@ -1861,52 +1861,52 @@
         <v>47</v>
       </c>
       <c r="I13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
         <v>37</v>
       </c>
       <c r="K13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s">
         <v>49</v>
       </c>
       <c r="M13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O13" t="s">
+        <v>120</v>
+      </c>
+      <c r="P13" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q13" t="s">
         <v>122</v>
       </c>
-      <c r="P13" t="s">
+      <c r="T13" t="s">
         <v>123</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="U13" t="s">
         <v>124</v>
       </c>
-      <c r="T13" t="s">
+      <c r="V13" t="s">
         <v>125</v>
-      </c>
-      <c r="U13" t="s">
-        <v>126</v>
-      </c>
-      <c r="V13" t="s">
-        <v>127</v>
       </c>
       <c r="Z13" t="s">
         <v>45</v>
       </c>
       <c r="AA13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AD13" t="s">
         <v>52</v>
       </c>
       <c r="AJ13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1">
         <v>41682</v>
@@ -1926,16 +1926,16 @@
         <v>41682</v>
       </c>
       <c r="F14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H14" t="s">
         <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L14" t="s">
         <v>49</v>
@@ -1944,31 +1944,31 @@
         <v>50</v>
       </c>
       <c r="N14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O14" t="s">
+        <v>100</v>
+      </c>
+      <c r="P14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q14" t="s">
         <v>102</v>
       </c>
-      <c r="P14" t="s">
+      <c r="T14" t="s">
         <v>103</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="U14" t="s">
         <v>104</v>
       </c>
-      <c r="T14" t="s">
+      <c r="V14" t="s">
         <v>105</v>
-      </c>
-      <c r="U14" t="s">
-        <v>106</v>
-      </c>
-      <c r="V14" t="s">
-        <v>107</v>
       </c>
       <c r="Z14" t="s">
         <v>45</v>
       </c>
       <c r="AA14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AD14" t="s">
         <v>52</v>
@@ -1979,7 +1979,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C15" s="3">
         <v>41638</v>
@@ -1991,7 +1991,7 @@
         <v>41647</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
         <v>47</v>
@@ -2003,31 +2003,31 @@
         <v>50</v>
       </c>
       <c r="N15" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="O15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" t="s">
         <v>76</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="T15" t="s">
+        <v>66</v>
+      </c>
+      <c r="U15" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" t="s">
         <v>78</v>
-      </c>
-      <c r="T15" t="s">
-        <v>67</v>
-      </c>
-      <c r="U15" t="s">
-        <v>68</v>
-      </c>
-      <c r="V15" t="s">
-        <v>79</v>
       </c>
       <c r="Z15" t="s">
         <v>45</v>
       </c>
       <c r="AA15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AD15" t="s">
         <v>52</v>
@@ -2038,7 +2038,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C16" s="1">
         <v>41974</v>
@@ -2056,13 +2056,13 @@
         <v>47</v>
       </c>
       <c r="I16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J16" t="s">
         <v>37</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L16" t="s">
         <v>49</v>
@@ -2074,10 +2074,10 @@
         <v>51</v>
       </c>
       <c r="O16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Q16" t="s">
         <v>55</v>
@@ -2092,10 +2092,10 @@
         <v>58</v>
       </c>
       <c r="X16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Y16" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Z16" t="s">
         <v>45</v>
@@ -2104,7 +2104,7 @@
         <v>59</v>
       </c>
       <c r="AB16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AD16" t="s">
         <v>52</v>
@@ -2115,7 +2115,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C17" s="1">
         <v>41974</v>
@@ -2136,7 +2136,7 @@
         <v>37</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L17" t="s">
         <v>49</v>
@@ -2148,16 +2148,16 @@
         <v>51</v>
       </c>
       <c r="O17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Q17" t="s">
         <v>55</v>
       </c>
       <c r="R17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="T17" t="s">
         <v>56</v>
@@ -2169,13 +2169,13 @@
         <v>58</v>
       </c>
       <c r="W17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="X17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Y17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Z17" t="s">
         <v>45</v>
@@ -2184,7 +2184,7 @@
         <v>59</v>
       </c>
       <c r="AB17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AD17" t="s">
         <v>52</v>

</xml_diff>